<commit_message>
Added OpenPM8546 PROMs. Handle LG Increment/query. Add more comments
</commit_message>
<xml_diff>
--- a/PM5644/PM8546/Docs/BOM_8546.xlsx
+++ b/PM5644/PM8546/Docs/BOM_8546.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Electronics\TV\PM5644\PM8546\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBFFC52-66F8-44B8-8BB6-C75DA190065E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8432035B-C4A1-4E2C-9CE7-C639ED32E33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="372">
   <si>
     <t>D1</t>
   </si>
@@ -1137,22 +1137,10 @@
     <t>G23270006</t>
   </si>
   <si>
-    <t>1-2199298-3</t>
-  </si>
-  <si>
-    <t>CONN IC DIP SOCKET 14POS TIN</t>
-  </si>
-  <si>
-    <t>Solder part directly to PCB</t>
-  </si>
-  <si>
-    <t>OPTIONAL</t>
-  </si>
-  <si>
-    <t>Socket chip. Optional in 16:9 version.</t>
-  </si>
-  <si>
     <t>PCB connector</t>
+  </si>
+  <si>
+    <t>74F164/SN74ALS164AN</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F231"/>
+  <dimension ref="A1:F228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C214" sqref="C214:C219"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D229" sqref="D229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4386,7 +4374,7 @@
         <v>268</v>
       </c>
       <c r="D198" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E198" t="s">
         <v>269</v>
@@ -4403,7 +4391,7 @@
         <v>268</v>
       </c>
       <c r="D199" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E199" t="s">
         <v>269</v>
@@ -4420,7 +4408,7 @@
         <v>268</v>
       </c>
       <c r="D200" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E200" t="s">
         <v>269</v>
@@ -4646,7 +4634,7 @@
         <v>269</v>
       </c>
       <c r="F214" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -4663,7 +4651,7 @@
         <v>269</v>
       </c>
       <c r="F215" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -4804,7 +4792,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>113</v>
       </c>
@@ -4818,7 +4806,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>115</v>
       </c>
@@ -4832,7 +4820,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>128</v>
       </c>
@@ -4846,7 +4834,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>129</v>
       </c>
@@ -4858,66 +4846,6 @@
       </c>
       <c r="E228" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>125</v>
-      </c>
-      <c r="B229" t="s">
-        <v>371</v>
-      </c>
-      <c r="C229" t="s">
-        <v>372</v>
-      </c>
-      <c r="D229" t="s">
-        <v>370</v>
-      </c>
-      <c r="E229" t="s">
-        <v>269</v>
-      </c>
-      <c r="F229" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>126</v>
-      </c>
-      <c r="B230" t="s">
-        <v>371</v>
-      </c>
-      <c r="C230" t="s">
-        <v>372</v>
-      </c>
-      <c r="D230" t="s">
-        <v>370</v>
-      </c>
-      <c r="E230" t="s">
-        <v>269</v>
-      </c>
-      <c r="F230" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>127</v>
-      </c>
-      <c r="B231" t="s">
-        <v>371</v>
-      </c>
-      <c r="C231" t="s">
-        <v>372</v>
-      </c>
-      <c r="D231" t="s">
-        <v>370</v>
-      </c>
-      <c r="E231" t="s">
-        <v>269</v>
-      </c>
-      <c r="F231" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>